<commit_message>
export sales invoice via excel
</commit_message>
<xml_diff>
--- a/DAChuyenNganh/wwwroot/templates/BillTemplate.xlsx
+++ b/DAChuyenNganh/wwwroot/templates/BillTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DA_ChuyenNganh\DAChuyenNganh\DAChuyenNganh\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B00208-2FE4-412B-BB2D-D84680182D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A8DF62-514B-434F-8B70-0C96062A03EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,17 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,9 +41,6 @@
     <t>Ngày ......... tháng ......... năm 20.........</t>
   </si>
   <si>
-    <t>SĐT: 0966 026 626</t>
-  </si>
-  <si>
     <t>Địa chỉ :  331 Quốc Lộ 1A an phú đông
 ĐT: 0966 036 626</t>
   </si>
@@ -68,6 +76,9 @@
   </si>
   <si>
     <t>Người lập hóa đơn</t>
+  </si>
+  <si>
+    <t>SĐT: 123 456 789</t>
   </si>
 </sst>
 </file>
@@ -313,22 +324,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
+      <xdr:colOff>368300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1619251</xdr:colOff>
+      <xdr:colOff>1955882</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>828676</xdr:rowOff>
+      <xdr:rowOff>742983</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{484D9AC7-CC6F-4D83-A439-9F12BFB37BD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -337,7 +348,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -350,8 +361,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1181100" y="19050"/>
-          <a:ext cx="809626" cy="809626"/>
+          <a:off x="755650" y="107950"/>
+          <a:ext cx="1587582" cy="635033"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -628,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:E29"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -645,14 +656,14 @@
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
       <c r="C1" s="20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -661,13 +672,13 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="18"/>
@@ -676,7 +687,7 @@
     </row>
     <row r="5" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18"/>
@@ -685,7 +696,7 @@
     </row>
     <row r="6" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -697,16 +708,16 @@
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,7 +902,7 @@
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="3">
@@ -920,11 +931,11 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>

</xml_diff>